<commit_message>
Included minimum number of  under 18's in grade download and impor
</commit_message>
<xml_diff>
--- a/test/fixtures/files/grade.xlsx
+++ b/test/fixtures/files/grade.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">RowID</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">MinFemales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinU18</t>
   </si>
   <si>
     <t xml:space="preserve">TeamSize</t>
@@ -101,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -186,13 +190,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.68"/>
@@ -200,16 +204,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -261,25 +265,28 @@
       <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>-2004596727</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>130</v>
@@ -288,7 +295,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>999</v>
@@ -303,12 +310,15 @@
         <v>3</v>
       </c>
       <c r="N2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="P2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="Q2" s="0" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update grade import to match on either RowID or Name
</commit_message>
<xml_diff>
--- a/test/fixtures/files/grade.xlsx
+++ b/test/fixtures/files/grade.xlsx
@@ -193,10 +193,10 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.68"/>
@@ -204,7 +204,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.38"/>
@@ -271,7 +271,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>-2004596727</v>
+        <v>202401</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Sport numbers can nnow be limited by grade as well as by overall sport
</commit_message>
<xml_diff>
--- a/test/fixtures/files/grade.xlsx
+++ b/test/fixtures/files/grade.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">RowID</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxIndivGrp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxTeamGrp</t>
   </si>
   <si>
     <t xml:space="preserve">MaxAge</t>
@@ -190,13 +196,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.68"/>
@@ -204,16 +210,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="5.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,57 +276,63 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>202401</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>999</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="O2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="P2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="Q2" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="R2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="S2" s="0" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>